<commit_message>
fix: :bug: Fixed .xlsx configuration import
</commit_message>
<xml_diff>
--- a/tests/material/configuration/xlsx/dates.xlsx
+++ b/tests/material/configuration/xlsx/dates.xlsx
@@ -31,10 +31,10 @@
     <t xml:space="preserve">rules.required</t>
   </si>
   <si>
-    <t xml:space="preserve">rules.minimum</t>
-  </si>
-  <si>
-    <t xml:space="preserve">rules.maximum</t>
+    <t xml:space="preserve">rules.dateMinimum</t>
+  </si>
+  <si>
+    <t xml:space="preserve">rules.dateMaximum</t>
   </si>
   <si>
     <t xml:space="preserve">controls</t>
@@ -276,7 +276,7 @@
   <dimension ref="A1:I2"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E8" activeCellId="0" sqref="E8"/>
+      <selection pane="topLeft" activeCell="G9" activeCellId="0" sqref="G9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>